<commit_message>
PRJ0018286- CF Industry Group Changes TECH changes 1st
</commit_message>
<xml_diff>
--- a/TestData/T1426_OpportunityToEngagementConversionMappingForCFJobTypes2.xlsx
+++ b/TestData/T1426_OpportunityToEngagementConversionMappingForCFJobTypes2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4666656-3B6E-41CD-94B4-C9C9CA3E7AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19AC0DC-CA7C-4D8B-8B8D-98ECD018F389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="85">
   <si>
     <t>Client</t>
   </si>
@@ -274,6 +274,15 @@
   </si>
   <si>
     <t>9999</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Post Merger Integration</t>
+  </si>
+  <si>
+    <t>Valuation Advisory</t>
   </si>
 </sst>
 </file>
@@ -667,7 +676,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyFont="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyFont="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -676,6 +685,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -998,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AF21" sqref="AF21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1951,6 +1963,282 @@
         <v>78</v>
       </c>
     </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="U11" t="s">
+        <v>30</v>
+      </c>
+      <c r="V11" t="s">
+        <v>69</v>
+      </c>
+      <c r="W11" t="s">
+        <v>33</v>
+      </c>
+      <c r="X11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S12" t="s">
+        <v>27</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="U12" t="s">
+        <v>30</v>
+      </c>
+      <c r="V12" t="s">
+        <v>69</v>
+      </c>
+      <c r="W12" t="s">
+        <v>33</v>
+      </c>
+      <c r="X12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>67</v>
+      </c>
+      <c r="M13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" t="s">
+        <v>71</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="U13" t="s">
+        <v>30</v>
+      </c>
+      <c r="V13" t="s">
+        <v>69</v>
+      </c>
+      <c r="W13" t="s">
+        <v>33</v>
+      </c>
+      <c r="X13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2072,10 +2360,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,6 +2514,48 @@
         <v>79</v>
       </c>
     </row>
+    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
changes Sept 27 2023
</commit_message>
<xml_diff>
--- a/TestData/T1426_OpportunityToEngagementConversionMappingForCFJobTypes2.xlsx
+++ b/TestData/T1426_OpportunityToEngagementConversionMappingForCFJobTypes2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19AC0DC-CA7C-4D8B-8B8D-98ECD018F389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074B787-5B9D-4D60-9F02-389D96476A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28950" windowHeight="14580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -1010,15 +1010,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD13"/>
+  <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
@@ -1043,7 +1044,7 @@
     <col min="30" max="30" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1135,7 +1136,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1226,8 +1227,11 @@
       <c r="AD2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1235,7 +1239,7 @@
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1318,8 +1322,11 @@
       <c r="AD3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1327,7 +1334,7 @@
         <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1410,8 +1417,11 @@
       <c r="AD4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1419,7 +1429,7 @@
         <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1502,8 +1512,11 @@
       <c r="AD5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1511,7 +1524,7 @@
         <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1594,8 +1607,11 @@
       <c r="AD6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -1603,7 +1619,7 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1686,8 +1702,11 @@
       <c r="AD7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>68</v>
       </c>
@@ -1695,7 +1714,7 @@
         <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1778,16 +1797,19 @@
       <c r="AD8" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE8" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>68</v>
       </c>
       <c r="B9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" t="s">
-        <v>66</v>
+      <c r="C9" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1865,21 +1887,24 @@
         <v>80</v>
       </c>
       <c r="AC9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>68</v>
       </c>
       <c r="B10" t="s">
         <v>68</v>
       </c>
-      <c r="C10" t="s">
-        <v>79</v>
+      <c r="C10" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1962,8 +1987,11 @@
       <c r="AD10" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1971,7 +1999,7 @@
         <v>68</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -2054,16 +2082,19 @@
       <c r="AD11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE11" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
       <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>83</v>
+      <c r="C12" t="s">
+        <v>73</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -2146,16 +2177,19 @@
       <c r="AD12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
       <c r="B13" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>84</v>
+      <c r="C13" t="s">
+        <v>74</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -2233,10 +2267,13 @@
         <v>80</v>
       </c>
       <c r="AC13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AD13" t="s">
-        <v>78</v>
+        <v>9</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2360,10 +2397,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2374,7 +2411,7 @@
     <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
@@ -2388,35 +2425,41 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>75</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
+        <v>55</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>56</v>
       </c>
@@ -2427,10 +2470,13 @@
         <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>56</v>
       </c>
@@ -2441,10 +2487,13 @@
         <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>56</v>
       </c>
@@ -2455,10 +2504,13 @@
         <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>56</v>
       </c>
@@ -2469,52 +2521,64 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="D9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>56</v>
       </c>
@@ -2525,35 +2589,44 @@
         <v>67</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>84</v>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EBITDA T1592 and T1426
</commit_message>
<xml_diff>
--- a/TestData/T1426_OpportunityToEngagementConversionMappingForCFJobTypes2.xlsx
+++ b/TestData/T1426_OpportunityToEngagementConversionMappingForCFJobTypes2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4074B787-5B9D-4D60-9F02-389D96476A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6A60F8-5658-40EE-A866-962583DCD60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28950" windowHeight="14580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="14610" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -1013,7 +1013,7 @@
   <dimension ref="A1:AE13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1144,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1222,13 +1222,13 @@
         <v>80</v>
       </c>
       <c r="AC2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AD2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE2">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -1239,7 +1239,7 @@
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1317,13 +1317,13 @@
         <v>80</v>
       </c>
       <c r="AC3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD3" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>4</v>
+        <v>78</v>
+      </c>
+      <c r="AE3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -1334,7 +1334,7 @@
         <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1412,13 +1412,13 @@
         <v>80</v>
       </c>
       <c r="AC4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AD4" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="AE4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -1429,7 +1429,7 @@
         <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1507,13 +1507,13 @@
         <v>80</v>
       </c>
       <c r="AC5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD5" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="AE5" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -1524,7 +1524,7 @@
         <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1602,13 +1602,13 @@
         <v>80</v>
       </c>
       <c r="AC6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AD6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE6">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1697,13 +1697,13 @@
         <v>80</v>
       </c>
       <c r="AC7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE7" s="1">
-        <v>8</v>
+        <v>78</v>
+      </c>
+      <c r="AE7">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -1714,7 +1714,7 @@
         <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1792,13 +1792,13 @@
         <v>80</v>
       </c>
       <c r="AC8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AD8" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="AE8" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -1808,8 +1808,8 @@
       <c r="B9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>82</v>
+      <c r="C9" t="s">
+        <v>79</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1893,7 +1893,7 @@
         <v>78</v>
       </c>
       <c r="AE9" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -1904,7 +1904,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1987,8 +1987,8 @@
       <c r="AD10" t="s">
         <v>78</v>
       </c>
-      <c r="AE10">
-        <v>11</v>
+      <c r="AE10" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
         <v>68</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -2082,8 +2082,8 @@
       <c r="AD11" t="s">
         <v>78</v>
       </c>
-      <c r="AE11" s="1">
-        <v>12</v>
+      <c r="AE11">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -2093,8 +2093,8 @@
       <c r="B12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" t="s">
-        <v>73</v>
+      <c r="C12" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -2178,7 +2178,7 @@
         <v>78</v>
       </c>
       <c r="AE12" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -2189,7 +2189,7 @@
         <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -2267,13 +2267,13 @@
         <v>80</v>
       </c>
       <c r="AC13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD13" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="AE13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2400,7 +2400,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,21 +2425,21 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>56</v>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
+        <v>74</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2453,10 +2453,10 @@
         <v>67</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="1">
-        <v>4</v>
+        <v>55</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2470,10 +2470,10 @@
         <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2487,10 +2487,10 @@
         <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2504,10 +2504,10 @@
         <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6">
-        <v>7</v>
+        <v>64</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2521,10 +2521,10 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="1">
-        <v>8</v>
+        <v>65</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2532,33 +2532,33 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
       </c>
       <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>82</v>
+      <c r="D9" t="s">
+        <v>79</v>
       </c>
       <c r="E9" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2572,10 +2572,10 @@
         <v>67</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10">
-        <v>11</v>
+        <v>82</v>
+      </c>
+      <c r="E10" s="1">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2589,44 +2589,44 @@
         <v>67</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
         <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>